<commit_message>
Add multi-copy PDF printing and system config endpoint
Implemented support for generating PDF tickets with multiple copies by rendering each copy as a separate page. Added a new /api/system/config endpoint to expose server OS type for frontend logic. On Linux, PDFs are now returned to the browser for manual printing instead of attempting direct server-side printing. Improved error handling and logging for PDF generation and printing. Updated pdf_generator.py to accept a 'copies' parameter and generate the appropriate number of pages.
</commit_message>
<xml_diff>
--- a/daily_log.xlsx
+++ b/daily_log.xlsx
@@ -3317,7 +3317,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:R3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -3466,15 +3466,11 @@
       <c r="H2" t="n">
         <v>50</v>
       </c>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr">
         <is>
           <t>HECTOR</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr"/>
-      <c r="M2" t="inlineStr"/>
       <c r="N2" t="inlineStr">
         <is>
           <t>05/12/25</t>
@@ -3490,8 +3486,55 @@
           <t>13:53</t>
         </is>
       </c>
-      <c r="Q2" t="inlineStr"/>
-      <c r="R2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Compra</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>RAMA TABLADA</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>HLSD</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>15200</v>
+      </c>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>05/12/25</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>15:15</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr"/>
+      <c r="Q3" t="inlineStr"/>
+      <c r="R3" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>